<commit_message>
Added email alert parser and renderer
</commit_message>
<xml_diff>
--- a/src/test/resources/test-alerts.xlsx
+++ b/src/test/resources/test-alerts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="alert policies" sheetId="2" r:id="rId1"/>
-    <sheet name="alert condition" sheetId="5" r:id="rId2"/>
-    <sheet name="infra metric" sheetId="1" r:id="rId3"/>
-    <sheet name="infra host not reporting" sheetId="3" r:id="rId4"/>
-    <sheet name="infra process running" sheetId="4" r:id="rId5"/>
-    <sheet name="nrql" sheetId="6" r:id="rId6"/>
+    <sheet name="email channels" sheetId="7" r:id="rId1"/>
+    <sheet name="alert policies" sheetId="2" r:id="rId2"/>
+    <sheet name="alert condition" sheetId="5" r:id="rId3"/>
+    <sheet name="infra metric" sheetId="1" r:id="rId4"/>
+    <sheet name="infra host not reporting" sheetId="3" r:id="rId5"/>
+    <sheet name="infra process running" sheetId="4" r:id="rId6"/>
+    <sheet name="nrql" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="107">
   <si>
     <t>Alert Policy</t>
   </si>
@@ -318,13 +319,40 @@
   </si>
   <si>
     <t>SELECT uniqueCount(containerId) FROM ProcessSample WHERE `containerLabel_io.kubernetes.pod.name` LIKE 'cap-dcp-acquisition-%'</t>
+  </si>
+  <si>
+    <t>email-channel</t>
+  </si>
+  <si>
+    <t>Recipients</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>Bob Smith</t>
+  </si>
+  <si>
+    <t>john.doe@test.com</t>
+  </si>
+  <si>
+    <t>jane.doe@test.com</t>
+  </si>
+  <si>
+    <t>bob.smith@test.com</t>
+  </si>
+  <si>
+    <t>include JSON Attachment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +487,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -757,7 +793,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -800,8 +836,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -810,8 +847,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -845,6 +883,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1164,7 +1203,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="gerald_curley@hotmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" display="gerald_curley@hotmail.com" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A4" r:id="rId4" display="gerald_curley@hotmail.com" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{5156CC94-1413-41DA-9E8A-4A4F12CEAAB6}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{1969641C-8C8D-4AE1-9F92-CFBDF55A048B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1238,8 +1362,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1421,11 +1545,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2020,8 +2144,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2126,8 +2250,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2200,12 +2324,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added parsers and renderers for the rest of the alert channels
</commit_message>
<xml_diff>
--- a/src/test/resources/test-alerts.xlsx
+++ b/src/test/resources/test-alerts.xlsx
@@ -9,23 +9,30 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="email channels" sheetId="7" r:id="rId1"/>
-    <sheet name="alert policies" sheetId="2" r:id="rId2"/>
-    <sheet name="alert condition" sheetId="5" r:id="rId3"/>
-    <sheet name="infra metric" sheetId="1" r:id="rId4"/>
-    <sheet name="infra host not reporting" sheetId="3" r:id="rId5"/>
-    <sheet name="infra process running" sheetId="4" r:id="rId6"/>
-    <sheet name="nrql" sheetId="6" r:id="rId7"/>
+    <sheet name="slack channels" sheetId="8" r:id="rId2"/>
+    <sheet name="hipchat channels" sheetId="9" r:id="rId3"/>
+    <sheet name="campfire channels" sheetId="10" r:id="rId4"/>
+    <sheet name="opsgenie channels" sheetId="11" r:id="rId5"/>
+    <sheet name="pagerduty channels" sheetId="12" r:id="rId6"/>
+    <sheet name="victorops channels" sheetId="13" r:id="rId7"/>
+    <sheet name="xmatters channels" sheetId="14" r:id="rId8"/>
+    <sheet name="alert policies" sheetId="2" r:id="rId9"/>
+    <sheet name="alert condition" sheetId="5" r:id="rId10"/>
+    <sheet name="infra metric" sheetId="1" r:id="rId11"/>
+    <sheet name="infra host not reporting" sheetId="3" r:id="rId12"/>
+    <sheet name="infra process running" sheetId="4" r:id="rId13"/>
+    <sheet name="nrql" sheetId="6" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="169">
   <si>
     <t>Alert Policy</t>
   </si>
@@ -346,6 +353,192 @@
   </si>
   <si>
     <t>include JSON Attachment</t>
+  </si>
+  <si>
+    <t>#channel1</t>
+  </si>
+  <si>
+    <t>channel1</t>
+  </si>
+  <si>
+    <t>channel2</t>
+  </si>
+  <si>
+    <t>channel3</t>
+  </si>
+  <si>
+    <t>#channel3</t>
+  </si>
+  <si>
+    <t>#channel2</t>
+  </si>
+  <si>
+    <t>slack-channel</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>http://test1.com</t>
+  </si>
+  <si>
+    <t>http://test2.com</t>
+  </si>
+  <si>
+    <t>http://test3.com</t>
+  </si>
+  <si>
+    <t>Auth Token</t>
+  </si>
+  <si>
+    <t>Room ID</t>
+  </si>
+  <si>
+    <t>room1</t>
+  </si>
+  <si>
+    <t>room2</t>
+  </si>
+  <si>
+    <t>room3</t>
+  </si>
+  <si>
+    <t>hipchat-channel</t>
+  </si>
+  <si>
+    <t>XXXX-XXXX-0001</t>
+  </si>
+  <si>
+    <t>XXXX-XXXX-0002</t>
+  </si>
+  <si>
+    <t>XXXX-XXXX-0003</t>
+  </si>
+  <si>
+    <t>room-1</t>
+  </si>
+  <si>
+    <t>room-2</t>
+  </si>
+  <si>
+    <t>room-3</t>
+  </si>
+  <si>
+    <t>campfire-channel</t>
+  </si>
+  <si>
+    <t>Subdomain</t>
+  </si>
+  <si>
+    <t>domain.1</t>
+  </si>
+  <si>
+    <t>domain.2</t>
+  </si>
+  <si>
+    <t>domain.3</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>opsgenie-channel</t>
+  </si>
+  <si>
+    <t>API Key</t>
+  </si>
+  <si>
+    <t>Teams</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>tag1</t>
+  </si>
+  <si>
+    <t>tag2</t>
+  </si>
+  <si>
+    <t>tag3</t>
+  </si>
+  <si>
+    <t>recipient1</t>
+  </si>
+  <si>
+    <t>recipient2</t>
+  </si>
+  <si>
+    <t>recipient3</t>
+  </si>
+  <si>
+    <t>team1</t>
+  </si>
+  <si>
+    <t>team2</t>
+  </si>
+  <si>
+    <t>team3</t>
+  </si>
+  <si>
+    <t>XXX-002</t>
+  </si>
+  <si>
+    <t>XXX-001</t>
+  </si>
+  <si>
+    <t>XXX-003</t>
+  </si>
+  <si>
+    <t>service1</t>
+  </si>
+  <si>
+    <t>service2</t>
+  </si>
+  <si>
+    <t>service3</t>
+  </si>
+  <si>
+    <t>pagerduty-channel</t>
+  </si>
+  <si>
+    <t>Service Key</t>
+  </si>
+  <si>
+    <t>victorops-channel</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Route Key</t>
+  </si>
+  <si>
+    <t>ROUTE-001</t>
+  </si>
+  <si>
+    <t>ROUTE-002</t>
+  </si>
+  <si>
+    <t>ROUTE-003</t>
+  </si>
+  <si>
+    <t>xmatters-channel</t>
+  </si>
+  <si>
+    <t>x-channel1</t>
+  </si>
+  <si>
+    <t>x-channel2</t>
+  </si>
+  <si>
+    <t>x-channel3</t>
   </si>
 </sst>
 </file>
@@ -1206,7 +1399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1287,82 +1480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -1545,7 +1663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -2144,7 +2262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2250,7 +2368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2324,7 +2442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -2402,4 +2520,659 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11369160-41BF-4A6B-906D-69373D3A5A78}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9D69F23F-6928-4F49-A60F-E7B819CE1EFC}"/>
+    <hyperlink ref="C3:C4" r:id="rId2" display="http://test1.com" xr:uid="{0E83DD66-6471-4DC8-883F-77B79EC06DAB}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{9039B332-FFD7-45E3-A42C-9421EB9C3736}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{76FC9A83-E6B2-465F-AC2F-FF441737AACA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD40F91-A991-4126-B1CD-824EEEA5CFC6}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C913F9-7C3C-4465-9B72-BCE3B7FAE377}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{509306B4-004E-47AE-ADD3-B1389007D63B}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="38.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{335E86DA-D57F-4F6D-AD7F-711BE4B5A8CD}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="3" width="20.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE77CA6-3D64-452C-A05C-B440EFD432AA}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA21E60-8BF9-476B-A629-568D597A8161}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.88671875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9C05070F-DD3A-4C66-947F-4B440301265E}"/>
+    <hyperlink ref="C3:C4" r:id="rId2" display="http://test1.com" xr:uid="{493E4DE3-594E-4DA0-BE46-A31038655370}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{358FF9F7-8B55-4151-B856-326A5EB1BA80}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{D15B1C06-92F8-4572-82FF-6EE3A7A6C44A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added alert condition parser and renderer
</commit_message>
<xml_diff>
--- a/src/test/resources/test-alerts.xlsx
+++ b/src/test/resources/test-alerts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="email channels" sheetId="7" r:id="rId1"/>
@@ -21,18 +21,18 @@
     <sheet name="victorops channels" sheetId="13" r:id="rId7"/>
     <sheet name="xmatters channels" sheetId="14" r:id="rId8"/>
     <sheet name="alert policies" sheetId="2" r:id="rId9"/>
-    <sheet name="alert condition" sheetId="5" r:id="rId10"/>
-    <sheet name="infra metric" sheetId="1" r:id="rId11"/>
-    <sheet name="infra host not reporting" sheetId="3" r:id="rId12"/>
-    <sheet name="infra process running" sheetId="4" r:id="rId13"/>
-    <sheet name="nrql" sheetId="6" r:id="rId14"/>
+    <sheet name="alert conditions" sheetId="5" r:id="rId10"/>
+    <sheet name="infra metric conditions" sheetId="1" r:id="rId11"/>
+    <sheet name="infra host conditions" sheetId="3" r:id="rId12"/>
+    <sheet name="infra process conditions" sheetId="4" r:id="rId13"/>
+    <sheet name="nrql conditions" sheetId="6" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="172">
   <si>
     <t>Alert Policy</t>
   </si>
@@ -286,9 +286,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>Scope</t>
-  </si>
-  <si>
     <t>application</t>
   </si>
   <si>
@@ -539,6 +536,18 @@
   </si>
   <si>
     <t>x-channel3</t>
+  </si>
+  <si>
+    <t>Condition Scope</t>
+  </si>
+  <si>
+    <t>Condition Type</t>
+  </si>
+  <si>
+    <t>alert-condition</t>
+  </si>
+  <si>
+    <t>default-apm-policy</t>
   </si>
 </sst>
 </file>
@@ -1419,21 +1428,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1441,13 +1450,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1455,13 +1464,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1482,23 +1491,23 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.21875" customWidth="1"/>
-    <col min="5" max="5" width="38.88671875" customWidth="1"/>
-    <col min="10" max="10" width="22.88671875" customWidth="1"/>
+    <col min="3" max="4" width="17.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" customWidth="1"/>
+    <col min="6" max="6" width="38.88671875" customWidth="1"/>
+    <col min="11" max="11" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1509,28 +1518,31 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>84</v>
+        <v>169</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1538,31 +1550,34 @@
         <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>170</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G2">
+        <v>86</v>
+      </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2">
         <v>0.8</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.7</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1570,31 +1585,34 @@
         <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>170</v>
       </c>
       <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F3" t="s">
         <v>86</v>
       </c>
-      <c r="E3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3">
         <v>0.7</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.6</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -1602,31 +1620,34 @@
         <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>170</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.5</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -1634,27 +1655,30 @@
         <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>5</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2447,7 +2471,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2470,7 +2494,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
@@ -2490,19 +2514,19 @@
     </row>
     <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -2514,7 +2538,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2546,52 +2570,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
         <v>110</v>
-      </c>
-      <c r="B4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2630,52 +2654,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
         <v>124</v>
       </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
         <v>123</v>
       </c>
-      <c r="B4" t="s">
-        <v>124</v>
-      </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2708,64 +2732,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2799,76 +2823,76 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2899,40 +2923,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" t="s">
         <v>156</v>
       </c>
-      <c r="B4" t="s">
-        <v>157</v>
-      </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2964,52 +2988,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -3022,7 +3046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCA21E60-8BF9-476B-A629-568D597A8161}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3042,52 +3066,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
         <v>165</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3104,10 +3128,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3172,6 +3196,17 @@
         <v>54</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed alert condition parser and renderer for entity ids
</commit_message>
<xml_diff>
--- a/src/test/resources/test-alerts.xlsx
+++ b/src/test/resources/test-alerts.xlsx
@@ -27,12 +27,12 @@
     <sheet name="infra process conditions" sheetId="4" r:id="rId13"/>
     <sheet name="nrql conditions" sheetId="6" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="175">
   <si>
     <t>Alert Policy</t>
   </si>
@@ -301,9 +301,6 @@
     <t>below</t>
   </si>
   <si>
-    <t>Application Filter</t>
-  </si>
-  <si>
     <t>apm_app_metric</t>
   </si>
   <si>
@@ -548,6 +545,18 @@
   </si>
   <si>
     <t>default-apm-policy</t>
+  </si>
+  <si>
+    <t>%-server</t>
+  </si>
+  <si>
+    <t>xxx-%</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>%-%</t>
   </si>
 </sst>
 </file>
@@ -1428,21 +1437,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1450,13 +1459,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1464,13 +1473,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1493,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1518,10 +1527,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
@@ -1539,7 +1548,7 @@
         <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>89</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1550,10 +1559,10 @@
         <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
         <v>84</v>
@@ -1574,7 +1583,7 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1585,10 +1594,10 @@
         <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
         <v>85</v>
@@ -1609,7 +1618,7 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>83</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1620,10 +1629,10 @@
         <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
         <v>84</v>
@@ -1644,7 +1653,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>83</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1655,10 +1664,10 @@
         <v>82</v>
       </c>
       <c r="C5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E5" t="s">
         <v>85</v>
@@ -2494,7 +2503,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>13</v>
@@ -2514,16 +2523,16 @@
     </row>
     <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" t="s">
         <v>88</v>
@@ -2538,7 +2547,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2570,52 +2579,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" t="s">
         <v>109</v>
-      </c>
-      <c r="B4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2654,52 +2663,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
         <v>123</v>
       </c>
-      <c r="C2" t="s">
-        <v>124</v>
-      </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
         <v>122</v>
       </c>
-      <c r="B4" t="s">
-        <v>123</v>
-      </c>
       <c r="C4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2732,64 +2741,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2823,76 +2832,76 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>140</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2923,40 +2932,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
         <v>155</v>
       </c>
-      <c r="B4" t="s">
-        <v>156</v>
-      </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -2988,52 +2997,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3066,52 +3075,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
         <v>164</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3198,7 +3207,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Added channels column for alert policies
</commit_message>
<xml_diff>
--- a/src/test/resources/test-alerts.xlsx
+++ b/src/test/resources/test-alerts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="email channels" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="201">
   <si>
     <t>Alert Policy</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>infra-metric</t>
-  </si>
-  <si>
     <t>disk-used-percent</t>
   </si>
   <si>
@@ -206,39 +203,12 @@
     <t>commandName = 'java'</t>
   </si>
   <si>
-    <t>Host Filter</t>
-  </si>
-  <si>
-    <t>hostname LIKE 'aem-%'</t>
-  </si>
-  <si>
-    <t>Process Filter</t>
-  </si>
-  <si>
-    <t>aem-process-policy</t>
-  </si>
-  <si>
     <t>process-default-cpu-percent</t>
   </si>
   <si>
-    <t>commandName != 'java'</t>
-  </si>
-  <si>
     <t xml:space="preserve">default-host-policy	</t>
   </si>
   <si>
-    <t>host-basic-consumers-not-reporting</t>
-  </si>
-  <si>
-    <t>hostname LIKE 'basic-consumers-%'</t>
-  </si>
-  <si>
-    <t>host-complex-consumers-not-reporting</t>
-  </si>
-  <si>
-    <t>hostname LIKE 'complex-consumers-%'</t>
-  </si>
-  <si>
     <t>host-ui-not-reporting</t>
   </si>
   <si>
@@ -251,24 +221,12 @@
     <t>hostname LIKE 'client-%'</t>
   </si>
   <si>
-    <t>java-not-running</t>
-  </si>
-  <si>
-    <t>infra-host-not-reporting</t>
-  </si>
-  <si>
-    <t>infra-process-running</t>
-  </si>
-  <si>
     <t>Critical</t>
   </si>
   <si>
     <t>equal</t>
   </si>
   <si>
-    <t xml:space="preserve">aem-process-policy	</t>
-  </si>
-  <si>
     <t xml:space="preserve">default-apm-policy	</t>
   </si>
   <si>
@@ -311,15 +269,9 @@
     <t>hostname LIKE 'ip-%'</t>
   </si>
   <si>
-    <t>container-cap-dcp-acquisition-count</t>
-  </si>
-  <si>
     <t>Query</t>
   </si>
   <si>
-    <t>SELECT uniqueCount(containerId) FROM ProcessSample WHERE `containerLabel_io.kubernetes.pod.name` LIKE 'cap-dcp-acquisition-%'</t>
-  </si>
-  <si>
     <t>email-channel</t>
   </si>
   <si>
@@ -350,15 +302,6 @@
     <t>#channel1</t>
   </si>
   <si>
-    <t>channel1</t>
-  </si>
-  <si>
-    <t>channel2</t>
-  </si>
-  <si>
-    <t>channel3</t>
-  </si>
-  <si>
     <t>#channel3</t>
   </si>
   <si>
@@ -389,15 +332,6 @@
     <t>Room ID</t>
   </si>
   <si>
-    <t>room1</t>
-  </si>
-  <si>
-    <t>room2</t>
-  </si>
-  <si>
-    <t>room3</t>
-  </si>
-  <si>
     <t>hipchat-channel</t>
   </si>
   <si>
@@ -488,15 +422,6 @@
     <t>XXX-003</t>
   </si>
   <si>
-    <t>service1</t>
-  </si>
-  <si>
-    <t>service2</t>
-  </si>
-  <si>
-    <t>service3</t>
-  </si>
-  <si>
     <t>pagerduty-channel</t>
   </si>
   <si>
@@ -585,6 +510,132 @@
   </si>
   <si>
     <t>nrql-alert-condition</t>
+  </si>
+  <si>
+    <t>infra-metric-alert-condition</t>
+  </si>
+  <si>
+    <t>Comparison</t>
+  </si>
+  <si>
+    <t>app-process-policy</t>
+  </si>
+  <si>
+    <t>hostname LIKE 'app-%'</t>
+  </si>
+  <si>
+    <t>Where Clause</t>
+  </si>
+  <si>
+    <t>infra-process-alert-condition</t>
+  </si>
+  <si>
+    <t>infra-host-alert-condition</t>
+  </si>
+  <si>
+    <t>Process Where Clause</t>
+  </si>
+  <si>
+    <t>default-host-policy</t>
+  </si>
+  <si>
+    <t>SELECT uniqueCount(containerId) FROM ProcessSample WHERE `container.name` LIKE 'app-%'</t>
+  </si>
+  <si>
+    <t>container-app-count</t>
+  </si>
+  <si>
+    <t>host-app-not-reporting</t>
+  </si>
+  <si>
+    <t>host-database-not-reporting</t>
+  </si>
+  <si>
+    <t>hostname LIKE 'database-%'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app-process-policy	</t>
+  </si>
+  <si>
+    <t>app-java-not-running</t>
+  </si>
+  <si>
+    <t>ui-java-not-running</t>
+  </si>
+  <si>
+    <t>Channels</t>
+  </si>
+  <si>
+    <t>hb-room1</t>
+  </si>
+  <si>
+    <t>hb-room2</t>
+  </si>
+  <si>
+    <t>hb-room3</t>
+  </si>
+  <si>
+    <t>cf-channel1</t>
+  </si>
+  <si>
+    <t>cf-channel2</t>
+  </si>
+  <si>
+    <t>cf-channel3</t>
+  </si>
+  <si>
+    <t>og-channel1</t>
+  </si>
+  <si>
+    <t>og-channel2</t>
+  </si>
+  <si>
+    <t>og-channel3</t>
+  </si>
+  <si>
+    <t>pd-service1</t>
+  </si>
+  <si>
+    <t>pd-service2</t>
+  </si>
+  <si>
+    <t>pd-service3</t>
+  </si>
+  <si>
+    <t>vo-channel1</t>
+  </si>
+  <si>
+    <t>vo-channel2</t>
+  </si>
+  <si>
+    <t>vo-channel3</t>
+  </si>
+  <si>
+    <t>xm-channel1</t>
+  </si>
+  <si>
+    <t>xm-channel2</t>
+  </si>
+  <si>
+    <t>xm-channel3</t>
+  </si>
+  <si>
+    <t>sl-channel1</t>
+  </si>
+  <si>
+    <t>sl-channel2</t>
+  </si>
+  <si>
+    <t>sl-channel3</t>
+  </si>
+  <si>
+    <t>John Doe , sl-channel1</t>
+  </si>
+  <si>
+    <t>Jane Doe, sl-channel2</t>
+  </si>
+  <si>
+    <t>Bob Smith,sl-channel3</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1497,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1465,21 +1516,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1487,13 +1538,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1501,13 +1552,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1555,51 +1606,51 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="H2">
         <v>0.8</v>
@@ -1611,30 +1662,30 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="H3">
         <v>0.7</v>
@@ -1646,30 +1697,30 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4">
         <v>0.5</v>
@@ -1681,30 +1732,30 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1716,7 +1767,7 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1728,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2985D7C4-7D8B-4E4D-982C-949DCCFA2D7C}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1754,48 +1805,48 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1807,30 +1858,30 @@
         <v>5</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
       <c r="K2" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
       <c r="E3" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1842,10 +1893,10 @@
         <v>5</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="K3" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1859,24 +1910,24 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="15.21875" customWidth="1"/>
     <col min="5" max="5" width="38.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
     <col min="10" max="10" width="22.88671875" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1887,48 +1938,45 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" t="s">
         <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
       </c>
       <c r="G2">
         <v>80</v>
@@ -1940,24 +1988,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3">
         <v>20</v>
@@ -1969,24 +2017,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>20</v>
@@ -1998,24 +2046,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5">
         <v>20000000</v>
@@ -2024,24 +2072,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6">
         <v>2000000</v>
@@ -2050,24 +2098,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7">
         <v>20</v>
@@ -2076,24 +2124,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8">
         <v>20</v>
@@ -2102,24 +2150,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>29</v>
-      </c>
       <c r="E9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9">
         <v>80</v>
@@ -2131,24 +2179,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10">
         <v>10</v>
@@ -2160,24 +2208,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>159</v>
+      </c>
+      <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -2189,24 +2237,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>30</v>
@@ -2218,24 +2266,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13">
         <v>60</v>
@@ -2247,24 +2295,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14">
         <v>60</v>
@@ -2276,24 +2324,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>159</v>
+      </c>
+      <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
-        <v>42</v>
-      </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15">
         <v>40000000</v>
@@ -2302,24 +2350,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" t="s">
-        <v>42</v>
-      </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H16">
         <v>10000000</v>
@@ -2328,24 +2376,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D17" t="s">
         <v>41</v>
       </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" t="s">
-        <v>42</v>
-      </c>
       <c r="E17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H17">
         <v>5000</v>
@@ -2354,24 +2402,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" t="s">
         <v>41</v>
       </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
       <c r="E18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H18">
         <v>500</v>
@@ -2380,24 +2428,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19">
         <v>150</v>
@@ -2409,30 +2457,27 @@
         <v>20</v>
       </c>
       <c r="J19" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>161</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" t="s">
-        <v>61</v>
-      </c>
       <c r="C20" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20">
         <v>60</v>
@@ -2444,10 +2489,7 @@
         <v>20</v>
       </c>
       <c r="J20" t="s">
-        <v>58</v>
-      </c>
-      <c r="K20" t="s">
-        <v>62</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2461,7 +2503,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2483,78 +2525,78 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="D2">
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="D4">
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>165</v>
       </c>
       <c r="D5">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2564,10 +2606,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2575,8 +2617,9 @@
     <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="2" max="2" width="20.21875" customWidth="1"/>
     <col min="3" max="3" width="22.77734375" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -2590,33 +2633,33 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>160</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>166</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>174</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2625,10 +2668,36 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2664,39 +2733,39 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -2708,7 +2777,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2721,7 +2790,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2740,52 +2809,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2805,7 +2874,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2824,52 +2893,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2883,7 +2952,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2902,64 +2971,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" t="s">
         <v>106</v>
       </c>
-      <c r="B3" t="s">
-        <v>128</v>
-      </c>
       <c r="C3" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2973,7 +3042,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2993,76 +3062,76 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>183</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="F3" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3076,7 +3145,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3093,40 +3162,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3140,7 +3209,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3158,52 +3227,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>189</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="D2" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>190</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="D3" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="C4" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -3217,7 +3286,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3236,52 +3305,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
-        <v>163</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3298,10 +3367,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3309,9 +3378,10 @@
     <col min="1" max="1" width="21.77734375" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -3319,76 +3389,138 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="gerald_curley@hotmail.com" xr:uid="{E9BEABFF-3893-4AE2-9B45-2A17E9139CA9}"/>
+    <hyperlink ref="D3" r:id="rId2" display="gerald_curley@hotmail.com" xr:uid="{A527DF09-A50F-4C7A-AE58-A4F574BA237F}"/>
+    <hyperlink ref="D4" r:id="rId3" display="gerald_curley@hotmail.com" xr:uid="{9FB82791-2E6D-424F-98C4-09305395ADCA}"/>
+    <hyperlink ref="D5" r:id="rId4" display="gerald_curley@hotmail.com" xr:uid="{59A201A8-A0AF-4D40-BAC4-B783BEC2B5BA}"/>
+    <hyperlink ref="D6" r:id="rId5" display="gerald_curley@hotmail.com" xr:uid="{EE1F36D0-3F75-4204-A738-E029FF16E923}"/>
+    <hyperlink ref="D7" r:id="rId6" display="gerald_curley@hotmail.com" xr:uid="{6FE52004-E8B5-4B40-B7A8-99E7AE2A0B1F}"/>
+    <hyperlink ref="D8" r:id="rId7" display="gerald_curley@hotmail.com" xr:uid="{D239116E-5D21-48C3-8C2E-7C9AFA5D483E}"/>
+    <hyperlink ref="D9" r:id="rId8" display="gerald_curley@hotmail.com" xr:uid="{A41F3BF3-3EA3-48AF-989B-2FF9CCC3F510}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed ENTITIES column to contain list of entity names instead of ids Removed FILTER column from entity alert conditions
</commit_message>
<xml_diff>
--- a/src/test/resources/test-alerts.xlsx
+++ b/src/test/resources/test-alerts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="email channels" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="203">
   <si>
     <t>Alert Policy</t>
   </si>
@@ -242,9 +242,6 @@
     <t>error-percent-instance</t>
   </si>
   <si>
-    <t>%</t>
-  </si>
-  <si>
     <t>application</t>
   </si>
   <si>
@@ -479,9 +476,6 @@
     <t>Filter</t>
   </si>
   <si>
-    <t>%-%</t>
-  </si>
-  <si>
     <t>external-service-alert-condition</t>
   </si>
   <si>
@@ -636,6 +630,18 @@
   </si>
   <si>
     <t>Bob Smith,sl-channel3</t>
+  </si>
+  <si>
+    <t>Entities</t>
+  </si>
+  <si>
+    <t>%-server, %-% , emm-server</t>
+  </si>
+  <si>
+    <t>%-%, xxx-%</t>
+  </si>
+  <si>
+    <t>% , emm-server</t>
   </si>
 </sst>
 </file>
@@ -1516,21 +1522,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1538,13 +1544,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1552,13 +1558,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1581,8 +1587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1606,10 +1612,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -1627,7 +1633,7 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1638,19 +1644,19 @@
         <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H2">
         <v>0.8</v>
@@ -1662,7 +1668,7 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>145</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1673,19 +1679,19 @@
         <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
         <v>71</v>
       </c>
-      <c r="F3" t="s">
-        <v>72</v>
-      </c>
       <c r="G3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H3">
         <v>0.7</v>
@@ -1697,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>148</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1708,16 +1714,16 @@
         <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -1732,7 +1738,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -1743,16 +1749,16 @@
         <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -1767,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>69</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1779,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2985D7C4-7D8B-4E4D-982C-949DCCFA2D7C}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1805,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -1823,10 +1829,10 @@
         <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>147</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1834,16 +1840,16 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -1858,10 +1864,10 @@
         <v>5</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1869,16 +1875,16 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" t="s">
         <v>149</v>
-      </c>
-      <c r="D3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E3" t="s">
-        <v>151</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -1893,10 +1899,10 @@
         <v>5</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1944,7 +1950,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -1956,7 +1962,7 @@
         <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1967,7 +1973,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1996,7 +2002,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -2025,7 +2031,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -2054,7 +2060,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -2080,7 +2086,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -2106,7 +2112,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -2132,7 +2138,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -2158,7 +2164,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
@@ -2187,7 +2193,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
@@ -2216,7 +2222,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
@@ -2245,7 +2251,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
@@ -2274,7 +2280,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -2303,7 +2309,7 @@
         <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -2332,7 +2338,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D15" t="s">
         <v>41</v>
@@ -2358,7 +2364,7 @@
         <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D16" t="s">
         <v>41</v>
@@ -2384,7 +2390,7 @@
         <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D17" t="s">
         <v>41</v>
@@ -2410,7 +2416,7 @@
         <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D18" t="s">
         <v>41</v>
@@ -2430,13 +2436,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
@@ -2457,18 +2463,18 @@
         <v>20</v>
       </c>
       <c r="J19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D20" t="s">
         <v>41</v>
@@ -2489,7 +2495,7 @@
         <v>20</v>
       </c>
       <c r="J20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2528,7 +2534,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2536,16 +2542,16 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2">
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2553,16 +2559,16 @@
         <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2573,7 +2579,7 @@
         <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -2590,7 +2596,7 @@
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -2633,7 +2639,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>62</v>
@@ -2642,21 +2648,21 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -2671,18 +2677,18 @@
         <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" t="s">
         <v>173</v>
       </c>
-      <c r="B3" t="s">
-        <v>175</v>
-      </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
@@ -2733,7 +2739,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>12</v>
@@ -2748,24 +2754,24 @@
         <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -2777,7 +2783,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2809,52 +2815,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2893,52 +2899,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
         <v>99</v>
       </c>
-      <c r="C2" t="s">
-        <v>100</v>
-      </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2971,64 +2977,64 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3062,76 +3068,76 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3162,40 +3168,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -3227,52 +3233,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3305,52 +3311,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
         <v>137</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3369,7 +3375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -3392,7 +3398,7 @@
         <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3406,7 +3412,7 @@
         <v>53</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3420,7 +3426,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3434,7 +3440,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3448,12 +3454,12 @@
         <v>53</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
@@ -3462,12 +3468,12 @@
         <v>53</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -3476,12 +3482,12 @@
         <v>53</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -3490,12 +3496,12 @@
         <v>53</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
         <v>50</v>
@@ -3504,7 +3510,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added the rest of the infra conditions to AlertManager
</commit_message>
<xml_diff>
--- a/src/test/resources/test-alerts.xlsx
+++ b/src/test/resources/test-alerts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5052" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="email channels" sheetId="7" r:id="rId1"/>
@@ -497,12 +497,6 @@
     <t>External Service URL</t>
   </si>
   <si>
-    <t>http://test.co.uk</t>
-  </si>
-  <si>
-    <t>http://test.com</t>
-  </si>
-  <si>
     <t>nrql-alert-condition</t>
   </si>
   <si>
@@ -642,6 +636,12 @@
   </si>
   <si>
     <t>% , emm-server</t>
+  </si>
+  <si>
+    <t>test.com</t>
+  </si>
+  <si>
+    <t>test.co.uk</t>
   </si>
 </sst>
 </file>
@@ -1587,7 +1587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -1633,7 +1633,7 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1668,7 +1668,7 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -1703,7 +1703,7 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1773,7 +1773,7 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1785,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2985D7C4-7D8B-4E4D-982C-949DCCFA2D7C}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1832,7 +1832,7 @@
         <v>153</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1864,7 +1864,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>155</v>
+        <v>201</v>
       </c>
       <c r="K2" t="s">
         <v>144</v>
@@ -1899,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="K3" t="s">
         <v>145</v>
@@ -1907,8 +1907,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{D606C31B-3E84-4F13-A2F4-C035499CEEA6}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{28BD1B97-1700-4702-9807-596A65620D7C}"/>
+    <hyperlink ref="J2" r:id="rId1" display="http://test.com" xr:uid="{D606C31B-3E84-4F13-A2F4-C035499CEEA6}"/>
+    <hyperlink ref="J3" r:id="rId2" display="http://test.co.uk" xr:uid="{28BD1B97-1700-4702-9807-596A65620D7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1950,7 +1950,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>14</v>
@@ -1962,7 +1962,7 @@
         <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1973,7 +1973,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -2002,7 +2002,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -2031,7 +2031,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -2060,7 +2060,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -2086,7 +2086,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -2112,7 +2112,7 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -2138,7 +2138,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
         <v>22</v>
@@ -2164,7 +2164,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
         <v>28</v>
@@ -2193,7 +2193,7 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
@@ -2222,7 +2222,7 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D11" t="s">
         <v>28</v>
@@ -2251,7 +2251,7 @@
         <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D12" t="s">
         <v>28</v>
@@ -2280,7 +2280,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D13" t="s">
         <v>28</v>
@@ -2309,7 +2309,7 @@
         <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D14" t="s">
         <v>41</v>
@@ -2338,7 +2338,7 @@
         <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D15" t="s">
         <v>41</v>
@@ -2364,7 +2364,7 @@
         <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D16" t="s">
         <v>41</v>
@@ -2390,7 +2390,7 @@
         <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
         <v>41</v>
@@ -2416,7 +2416,7 @@
         <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D18" t="s">
         <v>41</v>
@@ -2436,13 +2436,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D19" t="s">
         <v>41</v>
@@ -2463,18 +2463,18 @@
         <v>20</v>
       </c>
       <c r="J19" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B20" t="s">
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D20" t="s">
         <v>41</v>
@@ -2495,7 +2495,7 @@
         <v>20</v>
       </c>
       <c r="J20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2534,7 +2534,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -2542,16 +2542,16 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D2">
         <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2559,16 +2559,16 @@
         <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D3">
         <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2579,7 +2579,7 @@
         <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -2596,7 +2596,7 @@
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -2639,7 +2639,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>62</v>
@@ -2648,21 +2648,21 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D2" t="s">
         <v>63</v>
@@ -2677,18 +2677,18 @@
         <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" t="s">
         <v>171</v>
       </c>
-      <c r="B3" t="s">
-        <v>173</v>
-      </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
         <v>63</v>
@@ -2762,13 +2762,13 @@
         <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E2" t="s">
         <v>73</v>
@@ -2823,7 +2823,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B2" t="s">
         <v>90</v>
@@ -2837,7 +2837,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
         <v>90</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
         <v>90</v>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B2" t="s">
         <v>98</v>
@@ -2921,7 +2921,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
         <v>98</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B4" t="s">
         <v>98</v>
@@ -2988,7 +2988,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B2" t="s">
         <v>105</v>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
         <v>105</v>
@@ -3022,7 +3022,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B4" t="s">
         <v>105</v>
@@ -3082,7 +3082,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
@@ -3102,7 +3102,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s">
         <v>112</v>
@@ -3122,7 +3122,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
         <v>112</v>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2" t="s">
         <v>128</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
         <v>128</v>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B4" t="s">
         <v>128</v>
@@ -3241,7 +3241,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
         <v>130</v>
@@ -3269,7 +3269,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
         <v>130</v>
@@ -3319,7 +3319,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
         <v>136</v>
@@ -3333,7 +3333,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
         <v>136</v>
@@ -3347,7 +3347,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
         <v>136</v>
@@ -3398,7 +3398,7 @@
         <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3412,7 +3412,7 @@
         <v>53</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3426,7 +3426,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -3440,7 +3440,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3454,7 +3454,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3468,7 +3468,7 @@
         <v>53</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3482,12 +3482,12 @@
         <v>53</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
@@ -3496,12 +3496,12 @@
         <v>53</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
         <v>50</v>
@@ -3510,7 +3510,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>